<commit_message>
Changes in InputFormSubmit,JavaScriptAlertPage,JQueryDatePickBothJavaFiles MultipleSelectDropDownList
</commit_message>
<xml_diff>
--- a/Files/InputData.xlsx
+++ b/Files/InputData.xlsx
@@ -5,26 +5,63 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\indganesan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbanduch\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="1845" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11175" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="SingleEnterMessage" sheetId="4" r:id="rId1"/>
-    <sheet name="SumOfValid" sheetId="5" r:id="rId2"/>
-    <sheet name="SingleRadioBtn" sheetId="7" r:id="rId3"/>
-    <sheet name="DoubleRadioBtn" sheetId="8" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet name="TableDataSearch" sheetId="1" r:id="rId1"/>
+    <sheet name="SingleEnterMessage" sheetId="4" r:id="rId2"/>
+    <sheet name="SumOfValid" sheetId="5" r:id="rId3"/>
+    <sheet name="InputFormSubmit" sheetId="6" r:id="rId4"/>
+    <sheet name="SingleRadioBtn" sheetId="7" r:id="rId5"/>
+    <sheet name="DoubleRadioBtn" sheetId="8" r:id="rId6"/>
+    <sheet name="SingleEnterMessage (2)" sheetId="9" r:id="rId7"/>
+    <sheet name="SumOfValid (2)" sheetId="10" r:id="rId8"/>
+    <sheet name="SingleRadioBtn (2)" sheetId="11" r:id="rId9"/>
+    <sheet name="DoubleRadioBtn (2)" sheetId="12" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="59">
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>ka</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>as</t>
+  </si>
+  <si>
+    <t>da</t>
+  </si>
+  <si>
+    <t>NameTextBox</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
   <si>
     <t>END</t>
   </si>
@@ -72,6 +109,69 @@
   </si>
   <si>
     <t>Test Data_06</t>
+  </si>
+  <si>
+    <t>This is Project Description3</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>#163, FirstFlr, Doddanekundi</t>
+  </si>
+  <si>
+    <t>(900)800-1244</t>
+  </si>
+  <si>
+    <t>1email@email.com</t>
+  </si>
+  <si>
+    <t>lastName3</t>
+  </si>
+  <si>
+    <t>firstName3</t>
+  </si>
+  <si>
+    <t>This is Project Description2</t>
+  </si>
+  <si>
+    <t>Delaware</t>
+  </si>
+  <si>
+    <t>(900)800-1243</t>
+  </si>
+  <si>
+    <t>lastName2</t>
+  </si>
+  <si>
+    <t>firstName2</t>
+  </si>
+  <si>
+    <t>This is Project Description1</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>firstName1</t>
+  </si>
+  <si>
+    <t>Samuels</t>
+  </si>
+  <si>
+    <t>Will</t>
+  </si>
+  <si>
+    <t>sam</t>
+  </si>
+  <si>
+    <t>ba</t>
+  </si>
+  <si>
+    <t>ma</t>
   </si>
   <si>
     <t>Gender</t>
@@ -111,7 +211,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +223,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -145,14 +253,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -455,6 +571,768 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="5">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="5">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B13:B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>1002</v>
+      </c>
+      <c r="C3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>412</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>253</v>
+      </c>
+      <c r="C5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>6565</v>
+      </c>
+      <c r="C7">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="4">
+        <v>42655</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="2">
+        <v>9008001242</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1">
+        <v>12345</v>
+      </c>
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2">
+        <v>12346</v>
+      </c>
+      <c r="I2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3">
+        <v>12347</v>
+      </c>
+      <c r="I3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4">
+        <v>7</v>
+      </c>
+      <c r="I4">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -469,47 +1347,47 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -518,12 +1396,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,18 +1413,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -557,7 +1435,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>1002</v>
@@ -568,7 +1446,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>412</v>
@@ -579,7 +1457,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>253</v>
@@ -590,7 +1468,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>12</v>
@@ -601,7 +1479,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B7">
         <v>6565</v>
@@ -612,12 +1490,12 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -625,12 +1503,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,239 +1518,91 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>